<commit_message>
Requirements Other packages commit
</commit_message>
<xml_diff>
--- a/Software Requirements/Packages Requirements.xlsx
+++ b/Software Requirements/Packages Requirements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="123">
   <si>
     <t>Group</t>
   </si>
@@ -122,20 +122,6 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>Setups the variables for the engage run</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While Check_Value &lt; 5
-       Increment Check_Value + 1
-       If Check_Value = 2
-             Set Ex_Range_Distance_1 
-             Ex_Range_Distance_2 to max
-       If Check_Value = 3
-             Set Ex_Range_Distance_1 
-             Ex_Range_Distance_2 to min
-</t>
-  </si>
-  <si>
     <t>Failure</t>
   </si>
   <si>
@@ -143,10 +129,6 @@
   </si>
   <si>
     <t>Input a test Id to see if a failure occurred</t>
-  </si>
-  <si>
-    <t>Test_Id Local = Test_Id
-If Failure_Data_Structure(Tests_Id_Local) = True</t>
   </si>
   <si>
     <t>Hex_Value_Lock</t>
@@ -350,9 +332,6 @@
   </si>
   <si>
     <t>Monitor</t>
-  </si>
-  <si>
-    <t>Device</t>
   </si>
   <si>
     <t>Sets the density and radius of the Device</t>
@@ -397,7 +376,114 @@
     <t>Initialises Variables for different device settings</t>
   </si>
   <si>
-    <t>Setups up the monitor for run-through</t>
+    <t>Test_Id Local = Test_Id
+If Failure_Data_Structure(Tests_Id_Local) = True
+    return True
+else 
+    return False
+end if</t>
+  </si>
+  <si>
+    <t>Get_Release_State</t>
+  </si>
+  <si>
+    <t>Comms_Rx_Recieve</t>
+  </si>
+  <si>
+    <t>Comms_Tx_Send</t>
+  </si>
+  <si>
+    <t>Get_Weapon_Code_Lock</t>
+  </si>
+  <si>
+    <t>Read_And_Buffer_Sensor_Data</t>
+  </si>
+  <si>
+    <t>Porobability_Lock_Failure</t>
+  </si>
+  <si>
+    <t>Returns the release state of engine components</t>
+  </si>
+  <si>
+    <t>Case statement for receiving 64 bit messages</t>
+  </si>
+  <si>
+    <t>Case statement for sending 64 bit messages</t>
+  </si>
+  <si>
+    <t>Returns the state of various weapon states</t>
+  </si>
+  <si>
+    <t>Loads input sensor data to data structure</t>
+  </si>
+  <si>
+    <t>Calculates probability of all phase failures</t>
+  </si>
+  <si>
+    <t>Failures_Status</t>
+  </si>
+  <si>
+    <t>Abort</t>
+  </si>
+  <si>
+    <t>Log_Failure</t>
+  </si>
+  <si>
+    <t>Call_Failure_And_Details</t>
+  </si>
+  <si>
+    <t>Input a test Id to see if a failure occurred and all occurrence details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outputs a list of all failures for last run time </t>
+  </si>
+  <si>
+    <t>Shuts down all operations and logs all details</t>
+  </si>
+  <si>
+    <t>Logs a failure for the Test Id entered</t>
+  </si>
+  <si>
+    <t>Initialises variables for the engage run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starts Monitor set values </t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Read_Signal_To_Register_Data</t>
+  </si>
+  <si>
+    <t>Buffer_Signals</t>
+  </si>
+  <si>
+    <t>Read_1_Bit_Signal_Data</t>
+  </si>
+  <si>
+    <t>Reads the signal value and returns a boolean</t>
+  </si>
+  <si>
+    <t>Read_8_Bit_Signal_Data</t>
+  </si>
+  <si>
+    <t>Reads the signal value and returns a 8 bit value</t>
+  </si>
+  <si>
+    <t>Read_32_Bit_Register_Contents</t>
+  </si>
+  <si>
+    <t>Read_64_Bit_Register_Contents</t>
+  </si>
+  <si>
+    <t>Returns the contents of the register indexed by what bits are needed</t>
+  </si>
+  <si>
+    <t>Reads the register value for the signal entered</t>
+  </si>
+  <si>
+    <t>Loads read signals into the buffer register</t>
   </si>
 </sst>
 </file>
@@ -776,16 +862,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="52.140625" customWidth="1"/>
     <col min="5" max="5" width="47.140625" customWidth="1"/>
@@ -805,311 +891,517 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="368.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>78</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="368.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="6"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="6"/>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
       <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1200,7 +1492,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1217,7 +1509,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1234,7 +1526,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1251,7 +1543,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1268,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1285,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1326,7 +1618,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1407,13 +1699,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>500</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1470,13 +1762,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1484,10 +1776,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
@@ -1537,7 +1829,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1554,10 +1846,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1571,10 +1863,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1588,10 +1880,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1605,10 +1897,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1622,10 +1914,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1639,10 +1931,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update for Bubbless help
</commit_message>
<xml_diff>
--- a/Software Requirements/Packages Requirements.xlsx
+++ b/Software Requirements/Packages Requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procedures" sheetId="1" r:id="rId1"/>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1513,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,7 +1894,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>